<commit_message>
mapeamento ultimas vias, change view
</commit_message>
<xml_diff>
--- a/dados_tratados/vias_faixa_azul.xlsx
+++ b/dados_tratados/vias_faixa_azul.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\faixa-azul\dados_tratados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02877606-B7FB-4686-B432-0D9A017F3E5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4652E6D-94B5-4AE3-B3DF-F3263C3C4AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFEB5CA4-DDBF-4FD4-8A54-AAD114B03AEE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
   <si>
     <t>logradouro</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>AVENIDA AFONSO DESCRAGNOLE TAUNAY</t>
+  </si>
+  <si>
+    <t>COMPLEXO VIARIO AYRTON SENNA</t>
   </si>
 </sst>
 </file>
@@ -539,8 +542,8 @@
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1129,7 +1132,7 @@
         <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="C24">
         <v>30</v>
@@ -1155,7 +1158,7 @@
         <v>31</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C25">
         <v>30</v>

</xml_diff>

<commit_message>
faixas que ficaram para fora
</commit_message>
<xml_diff>
--- a/dados_tratados/vias_faixa_azul.xlsx
+++ b/dados_tratados/vias_faixa_azul.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\faixa-azul\dados_tratados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4652E6D-94B5-4AE3-B3DF-F3263C3C4AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6C3E4E-E933-4D72-8A2F-C8FDE19A9EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFEB5CA4-DDBF-4FD4-8A54-AAD114B03AEE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>logradouro</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>COMPLEXO VIARIO AYRTON SENNA</t>
+  </si>
+  <si>
+    <t>AVENIDA BRAZ LEME</t>
+  </si>
+  <si>
+    <t>AVENIDA ELISEU DE ALMEIDA</t>
   </si>
 </sst>
 </file>
@@ -539,11 +545,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A502A61E-16EB-41AD-B341-B6C3C66FD837}">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1236,68 +1242,56 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C28">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D28">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E28">
         <v>2024</v>
       </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28">
-        <v>7.4</v>
-      </c>
       <c r="I28">
         <v>23</v>
       </c>
       <c r="J28">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="C29">
-        <v>1</v>
+        <v>29</v>
       </c>
       <c r="D29">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E29">
         <v>2024</v>
       </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
       <c r="I29">
         <v>24</v>
       </c>
       <c r="J29">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -1308,25 +1302,28 @@
       <c r="E30">
         <v>2024</v>
       </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
       <c r="H30">
-        <v>2.4</v>
+        <v>7.4</v>
       </c>
       <c r="I30">
         <v>25</v>
       </c>
       <c r="J30">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="C31">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D31">
         <v>6</v>
@@ -1334,31 +1331,28 @@
       <c r="E31">
         <v>2024</v>
       </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
       <c r="G31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="I31">
         <v>26</v>
       </c>
       <c r="J31">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C32">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D32">
         <v>6</v>
@@ -1366,17 +1360,75 @@
       <c r="E32">
         <v>2024</v>
       </c>
-      <c r="G32">
-        <v>0</v>
-      </c>
       <c r="H32">
-        <v>1.7</v>
+        <v>2.4</v>
       </c>
       <c r="I32">
         <v>27</v>
       </c>
       <c r="J32">
         <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33">
+        <v>27</v>
+      </c>
+      <c r="D33">
+        <v>6</v>
+      </c>
+      <c r="E33">
+        <v>2024</v>
+      </c>
+      <c r="F33">
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="H33">
+        <v>5.5</v>
+      </c>
+      <c r="I33">
+        <v>28</v>
+      </c>
+      <c r="J33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34">
+        <v>27</v>
+      </c>
+      <c r="D34">
+        <v>6</v>
+      </c>
+      <c r="E34">
+        <v>2024</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>1.7</v>
+      </c>
+      <c r="I34">
+        <v>29</v>
+      </c>
+      <c r="J34">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
novo formato download infosiga
</commit_message>
<xml_diff>
--- a/dados_tratados/vias_faixa_azul.xlsx
+++ b/dados_tratados/vias_faixa_azul.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\faixa-azul\dados_tratados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F6C3E4E-E933-4D72-8A2F-C8FDE19A9EF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC91A813-01A1-4FAA-BEC0-B125B3ED84F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BFEB5CA4-DDBF-4FD4-8A54-AAD114B03AEE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="47">
   <si>
     <t>logradouro</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>AVENIDA ELISEU DE ALMEIDA</t>
+  </si>
+  <si>
+    <t>COMPLEXO VIARIO MARIA MALUF</t>
   </si>
 </sst>
 </file>
@@ -545,11 +548,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A502A61E-16EB-41AD-B341-B6C3C66FD837}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B20" sqref="B20"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1317,10 +1320,10 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C31">
         <v>1</v>
@@ -1331,12 +1334,6 @@
       <c r="E31">
         <v>2024</v>
       </c>
-      <c r="G31">
-        <v>1</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
       <c r="I31">
         <v>26</v>
       </c>
@@ -1346,10 +1343,10 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -1360,25 +1357,28 @@
       <c r="E32">
         <v>2024</v>
       </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
       <c r="H32">
-        <v>2.4</v>
+        <v>1</v>
       </c>
       <c r="I32">
         <v>27</v>
       </c>
       <c r="J32">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C33">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>6</v>
@@ -1386,28 +1386,22 @@
       <c r="E33">
         <v>2024</v>
       </c>
-      <c r="F33">
-        <v>1</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
       <c r="H33">
-        <v>5.5</v>
+        <v>2.4</v>
       </c>
       <c r="I33">
         <v>28</v>
       </c>
       <c r="J33">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C34">
         <v>27</v>
@@ -1418,16 +1412,48 @@
       <c r="E34">
         <v>2024</v>
       </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34">
-        <v>1.7</v>
+        <v>5.5</v>
       </c>
       <c r="I34">
         <v>29</v>
       </c>
       <c r="J34">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35">
+        <v>27</v>
+      </c>
+      <c r="D35">
+        <v>6</v>
+      </c>
+      <c r="E35">
+        <v>2024</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="H35">
+        <v>1.7</v>
+      </c>
+      <c r="I35">
+        <v>30</v>
+      </c>
+      <c r="J35">
         <v>15</v>
       </c>
     </row>

</xml_diff>